<commit_message>
Add file generator for String Table in Weintek (StringTable.xlsx)
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="95">
   <si>
     <t>Structs</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>PLCName</t>
+  </si>
+  <si>
+    <t>PLC_Sha_2</t>
+  </si>
+  <si>
+    <t>StringTable_ID</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1174,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1391,9 @@
       <c r="E6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="H6" t="s">
         <v>72</v>
       </c>
@@ -1417,6 +1425,12 @@
       </c>
       <c r="C7" s="1">
         <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
       </c>
       <c r="H7" t="s">
         <v>73</v>

</xml_diff>